<commit_message>
update `WhatsApp Web` elements
- patches to web elements that weren't working
- other minor patches to the code
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://proverservice01-my.sharepoint.com/personal/thiago_macedo_proverservice_com_br/Documents/ZapLine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prover User\Documents\GitHub\ZapLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F80E63E5FD0EE5CE7076EF637F6DEA0A7A50E345" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6BC90C8-D55A-416E-829F-9B89565AE1FA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7113075B-CAE2-424E-81D2-457B4A8D915E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LISTA PADRÃO" sheetId="2" r:id="rId1"/>
+    <sheet name="DEFAULT LIST" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,18 +33,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nº</t>
   </si>
   <si>
-    <t>Nome (Opcional)</t>
-  </si>
-  <si>
-    <t>Nº de Telefone</t>
-  </si>
-  <si>
-    <t>Enviado</t>
+    <t>Name (Optional)</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>Sempre salve e feche antes de prosseguir.</t>
+  </si>
+  <si>
+    <t>Para usar mais abas, copie esta.</t>
+  </si>
+  <si>
+    <t>Always save and close before proceeding.</t>
+  </si>
+  <si>
+    <t>To use more tabs, copy this one.</t>
   </si>
 </sst>
 </file>
@@ -55,8 +67,16 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="\(00\)\ 0\ 0000\-0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -95,6 +115,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,14 +172,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela1" displayName="Tabela1" ref="A1:D6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D6" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nº" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº" dataDxfId="5">
       <calculatedColumnFormula>ROW(A2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Nome (Opcional)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Nº de Telefone" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Enviado" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name (Optional)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Telephone" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sent" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -423,22 +447,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,23 +476,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f>ROW(A2)-1</f>
         <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f>ROW(A3)-1</f>
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f>ROW(A4)-1</f>
         <v>3</v>
@@ -476,23 +512,41 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f>ROW(A5)-1</f>
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f>ROW(A6)-1</f>
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
+      <c r="F6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F6:I6"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2:C6">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix `time` and `string comparison`
- Removes string comparison from `FILE_TEXT_INPUT`
- Extends `SYNC_TIME` to 5 minutes
- Extends `sheet.xlsx` name input
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B70D9C-2B7F-4C10-90DE-B4CA07733E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531ADC99-D82A-4233-8A97-0C987721DCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,23 +114,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <b/>
@@ -141,6 +132,21 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom"/>
@@ -169,12 +175,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D6" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº" dataDxfId="6">
       <calculatedColumnFormula>ROW(A2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name (Optional)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Telephone" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sent" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name (Optional)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Telephone" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sent" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -446,13 +452,13 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -476,6 +482,7 @@
         <f>ROW(A2)-1</f>
         <v>1</v>
       </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
       <c r="F2" s="4" t="s">
@@ -490,6 +497,7 @@
         <f>ROW(A3)-1</f>
         <v>2</v>
       </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
       <c r="F3" s="4" t="s">
@@ -504,6 +512,7 @@
         <f>ROW(A4)-1</f>
         <v>3</v>
       </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
@@ -512,6 +521,7 @@
         <f>ROW(A5)-1</f>
         <v>4</v>
       </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="F5" s="4" t="s">
@@ -526,6 +536,7 @@
         <f>ROW(A6)-1</f>
         <v>5</v>
       </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
       <c r="F6" s="4" t="s">
@@ -542,16 +553,16 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F6:I6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:C6">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D6">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"✔"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"✘"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C6">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
blocked contacts & ´active_element´
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531ADC99-D82A-4233-8A97-0C987721DCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FBFD90-293A-4B9E-8245-A4AB63A42608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEFAULT LIST" sheetId="1" r:id="rId1"/>
+    <sheet name="DEFAULT LIST (2)" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Nº</t>
   </si>
@@ -110,18 +111,18 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
     <dxf>
       <font>
         <b/>
@@ -146,7 +147,27 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom"/>
@@ -154,6 +175,23 @@
     <dxf>
       <numFmt numFmtId="165" formatCode="\(00\)\ 0\ 0000\-0000"/>
       <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="\(00\)\ 0\ 0000\-0000"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" shrinkToFit="1"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0000"/>
@@ -175,12 +213,26 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D6" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nº" dataDxfId="13">
       <calculatedColumnFormula>ROW(A2)-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name (Optional)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Telephone" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sent" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name (Optional)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Telephone" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sent" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62777823-A177-4DE7-9D54-530868D870E4}" name="Tabela14" displayName="Tabela14" ref="A1:D6" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CFFA623B-8E9A-4D1C-9B9B-E9CD411CA452}" name="Nº" dataDxfId="9">
+      <calculatedColumnFormula>ROW(A2)-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{A33D2418-3933-47C7-BB99-6E9DBABB6CB3}" name="Name (Optional)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{77DB6688-1119-406F-8C70-2C2B244017B6}" name="Telephone" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6201A584-5A17-4A84-ADD2-8D59DEC5950D}" name="Sent" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,14 +503,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -482,37 +534,37 @@
         <f>ROW(A2)-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f>ROW(A3)-1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f>ROW(A4)-1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
@@ -521,30 +573,30 @@
         <f>ROW(A5)-1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f>ROW(A6)-1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -553,19 +605,144 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F6:I6"/>
   </mergeCells>
+  <conditionalFormatting sqref="B2:C6">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"✔"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"✘"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F00E9-5FC6-4C9F-B9F1-66D8F101ED8E}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <f>ROW(A2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A3)-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <f>ROW(A4)-1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <f>ROW(A5)-1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <f>ROW(A6)-1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D2:D6">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"✔"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"✘"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C6">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>